<commit_message>
MongoDb added to ConsoleClient
</commit_message>
<xml_diff>
--- a/CarsFactory.xlsx
+++ b/CarsFactory.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
-    <sheet name="CarTypes (Enum)" sheetId="4" r:id="rId2"/>
-    <sheet name="EngineTypes (Enum)" sheetId="2" r:id="rId3"/>
+    <sheet name="CarTypes" sheetId="4" r:id="rId2"/>
+    <sheet name="EngineTypes" sheetId="2" r:id="rId3"/>
     <sheet name="Manufacturers" sheetId="6" r:id="rId4"/>
     <sheet name="Dealers" sheetId="10" r:id="rId5"/>
     <sheet name="Addresses" sheetId="7" r:id="rId6"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
   <si>
     <t>ProductId</t>
   </si>
@@ -131,6 +131,129 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Plovdiv Enterprise</t>
+  </si>
+  <si>
+    <t>Varna CarsHeaven</t>
+  </si>
+  <si>
+    <t>Pleven Motorsport</t>
+  </si>
+  <si>
+    <t>Burgas MonserTruck</t>
+  </si>
+  <si>
+    <t>Pernik GolfGodfather</t>
+  </si>
+  <si>
+    <t>Vidin DreamworksMotorsport</t>
+  </si>
+  <si>
+    <t>Albena WestCoastMotors</t>
+  </si>
+  <si>
+    <t>Blagoevgrad ExtremeMotors</t>
+  </si>
+  <si>
+    <t>Ruse PlatinumMotorsport</t>
+  </si>
+  <si>
+    <t>Shumen UltimateCarsShop</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>Ferrari</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Plovdiv</t>
+  </si>
+  <si>
+    <t>Varna</t>
+  </si>
+  <si>
+    <t>Pleven</t>
+  </si>
+  <si>
+    <t>Burgas</t>
+  </si>
+  <si>
+    <t>Pernik</t>
+  </si>
+  <si>
+    <t>Vidin</t>
+  </si>
+  <si>
+    <t>Albena</t>
+  </si>
+  <si>
+    <t>Blagoevgrad</t>
+  </si>
+  <si>
+    <t>Ruse</t>
+  </si>
+  <si>
+    <t>Shumen</t>
+  </si>
+  <si>
+    <t>Porsche</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>str. Tsar Asen 33</t>
+  </si>
+  <si>
+    <t>str. Sredna Gora 4</t>
+  </si>
+  <si>
+    <t>bul. Maria Luiza 87</t>
+  </si>
+  <si>
+    <t>bul. Bulgaria 7</t>
+  </si>
+  <si>
+    <t>str. Aleko 9</t>
+  </si>
+  <si>
+    <t>str. Musala 1</t>
+  </si>
+  <si>
+    <t>bul. Ruski 8</t>
+  </si>
+  <si>
+    <t>str. Prespa 52</t>
+  </si>
+  <si>
+    <t>str. Rila 3</t>
+  </si>
+  <si>
+    <t>str. Tsar Simeon 12</t>
   </si>
 </sst>
 </file>
@@ -500,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +862,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,7 +937,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +989,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,30 +1042,48 @@
       <c r="A6" s="3">
         <v>5</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -955,13 +1096,13 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -977,51 +1118,111 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="C3" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="C4" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C5" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="C6" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="C7" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="C8" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="C9" s="3">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="C10" s="3">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="C11" s="3">
         <v>10</v>
       </c>
@@ -1036,13 +1237,13 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1061,49 +1262,109 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="3">
         <v>10</v>
       </c>
     </row>
@@ -1114,17 +1375,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1136,6 +1397,116 @@
       </c>
       <c r="C1" s="2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1145,15 +1516,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="1" max="2" width="12.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1162,6 +1533,46 @@
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Big merge: - MongoDB - working - JsonRepor - working - XmlReport - working - XmlLoader - working - CarsFactoryReportsClient - not working
</commit_message>
<xml_diff>
--- a/CarsFactory.xlsx
+++ b/CarsFactory.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
   <si>
     <t>ProductId</t>
   </si>
@@ -254,6 +254,36 @@
   </si>
   <si>
     <t>str. Tsar Simeon 12</t>
+  </si>
+  <si>
+    <t>BMW E93</t>
+  </si>
+  <si>
+    <t>Honda Integra Type R</t>
+  </si>
+  <si>
+    <t>BMW X5</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz CLK</t>
+  </si>
+  <si>
+    <t>Toyota GT86</t>
+  </si>
+  <si>
+    <t>BMW 5-Series E39</t>
+  </si>
+  <si>
+    <t>Audi A2</t>
+  </si>
+  <si>
+    <t>Toyota Hilux</t>
+  </si>
+  <si>
+    <t>Nissan GT-R</t>
+  </si>
+  <si>
+    <t>Toyota Prius</t>
   </si>
 </sst>
 </file>
@@ -298,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -317,6 +347,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,19 +655,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
     <col min="3" max="3" width="15" style="6" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
     <col min="9" max="9" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -669,51 +702,261 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>232</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2011</v>
+      </c>
+      <c r="H2" s="8">
+        <v>56000</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>156</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>1998</v>
+      </c>
+      <c r="H3" s="8">
+        <v>36000</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>188</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1999</v>
+      </c>
+      <c r="H4" s="8">
+        <v>44000</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>160</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>2008</v>
+      </c>
+      <c r="H5" s="8">
+        <v>68000</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>220</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>2012</v>
+      </c>
+      <c r="H6" s="8">
+        <v>130000</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>145</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1995</v>
+      </c>
+      <c r="H7" s="8">
+        <v>32000</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>89</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>1999</v>
+      </c>
+      <c r="H8" s="8">
+        <v>29000</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>166</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>1997</v>
+      </c>
+      <c r="H9" s="8">
+        <v>52000</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>356</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>2008</v>
+      </c>
+      <c r="H10" s="8">
+        <v>110000</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="9">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>68</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>2004</v>
+      </c>
+      <c r="H11" s="8">
+        <v>70000</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -817,6 +1060,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1096,7 +1340,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>